<commit_message>
new languages in data model
</commit_message>
<xml_diff>
--- a/data_model_files/daschland (daschland)/properties.xlsx
+++ b/data_model_files/daschland (daschland)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data_model_files/daschland (daschland)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data_model_files/daschland (daschland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304BA1A2-8042-4948-8C91-A15AE4B4F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEDF6DD-01F1-0947-8723-FE5630CB7CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="500" windowWidth="35120" windowHeight="23880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="500" windowWidth="59460" windowHeight="23880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,6 +103,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -120,6 +121,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -137,6 +139,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -155,6 +158,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -174,6 +178,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -192,6 +197,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -213,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="251">
   <si>
     <t>name</t>
   </si>
@@ -542,9 +548,6 @@
     <t>linkToFlyerID</t>
   </si>
   <si>
-    <t>Link to Flyer</t>
-  </si>
-  <si>
     <t>Link to Fairytale</t>
   </si>
   <si>
@@ -645,17 +648,348 @@
   </si>
   <si>
     <t>hasValue, schema:description</t>
+  </si>
+  <si>
+    <t>Anniversaire</t>
+  </si>
+  <si>
+    <t>Numéro de chapitre</t>
+  </si>
+  <si>
+    <t>Type de personnage</t>
+  </si>
+  <si>
+    <t>Droits d'auteur</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>Département</t>
+  </si>
+  <si>
+    <t>Description de l'article</t>
+  </si>
+  <si>
+    <t>Niveau d'éducation</t>
+  </si>
+  <si>
+    <t>Gâteau préféré</t>
+  </si>
+  <si>
+    <t>Nom du fichier</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Nom de famille</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>Animal de compagnie</t>
+  </si>
+  <si>
+    <t>Couleur de l'animal</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>Rôle</t>
+  </si>
+  <si>
+    <t>Numéro de page</t>
+  </si>
+  <si>
+    <t>Nom court</t>
+  </si>
+  <si>
+    <t>Espèce</t>
+  </si>
+  <si>
+    <t>Horodatage</t>
+  </si>
+  <si>
+    <t>Poids</t>
+  </si>
+  <si>
+    <t>Lieu du Pays des Merveilles</t>
+  </si>
+  <si>
+    <t>Partie de</t>
+  </si>
+  <si>
+    <t>Lien vers le personnage d'Alice</t>
+  </si>
+  <si>
+    <t>Lien vers le personnage animal</t>
+  </si>
+  <si>
+    <t>Lien vers l'ami animal</t>
+  </si>
+  <si>
+    <t>Lien vers Audio</t>
+  </si>
+  <si>
+    <t>Lien vers majordome</t>
+  </si>
+  <si>
+    <t>Lien vers le conte de fées</t>
+  </si>
+  <si>
+    <t>Lien vers la fiche d'information</t>
+  </si>
+  <si>
+    <t>Lien vers l'image</t>
+  </si>
+  <si>
+    <t>Lien vers le lieu</t>
+  </si>
+  <si>
+    <t>Link to Information Sheet</t>
+  </si>
+  <si>
+    <t>Lien vers la vidéo</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Compleanno</t>
+  </si>
+  <si>
+    <t>Numero del capitolo</t>
+  </si>
+  <si>
+    <t>Tipo di personaggio</t>
+  </si>
+  <si>
+    <t>Diritti dell'autore</t>
+  </si>
+  <si>
+    <t>Data di nascita</t>
+  </si>
+  <si>
+    <t>Dipartimento</t>
+  </si>
+  <si>
+    <t>Descrizione dell'articolo</t>
+  </si>
+  <si>
+    <t>Livello di istruzione</t>
+  </si>
+  <si>
+    <t>Torta preferita</t>
+  </si>
+  <si>
+    <t>Nome del file</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Genere</t>
+  </si>
+  <si>
+    <t>Cognome</t>
+  </si>
+  <si>
+    <t>Licenza</t>
+  </si>
+  <si>
+    <t>Animale domestico</t>
+  </si>
+  <si>
+    <t>Colore dell'animale</t>
+  </si>
+  <si>
+    <t>Citazione</t>
+  </si>
+  <si>
+    <t>Ruolo</t>
+  </si>
+  <si>
+    <t>Numero di pagina</t>
+  </si>
+  <si>
+    <t>Nome breve</t>
+  </si>
+  <si>
+    <t>Data e ora</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Posizione nel paese delle meraviglie</t>
+  </si>
+  <si>
+    <t>Parte di</t>
+  </si>
+  <si>
+    <t>Collegamento al personaggio di Alice</t>
+  </si>
+  <si>
+    <t>Collegamento al personaggio animale</t>
+  </si>
+  <si>
+    <t>Collegamento all'amico animale</t>
+  </si>
+  <si>
+    <t>Collegamento all'audio</t>
+  </si>
+  <si>
+    <t>Collegamento al maggiordomo</t>
+  </si>
+  <si>
+    <t>Collegamento alla fiaba</t>
+  </si>
+  <si>
+    <t>Collegamento alla scheda informativa</t>
+  </si>
+  <si>
+    <t>Collegamento all'immagine</t>
+  </si>
+  <si>
+    <t>Collegamento alla posizione</t>
+  </si>
+  <si>
+    <t>Collegamento al video</t>
+  </si>
+  <si>
+    <t>Stérilisé</t>
+  </si>
+  <si>
+    <t>Sterilizzato</t>
+  </si>
+  <si>
+    <t>Geburtstag</t>
+  </si>
+  <si>
+    <t>Kapitel Nummer</t>
+  </si>
+  <si>
+    <t>Zeichen-Typ</t>
+  </si>
+  <si>
+    <t>Urheberrecht</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Bildungsgrad</t>
+  </si>
+  <si>
+    <t>Lieblingskuchen</t>
+  </si>
+  <si>
+    <t>Name der Datei</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Geschlecht</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Lizenz</t>
+  </si>
+  <si>
+    <t>Haustier</t>
+  </si>
+  <si>
+    <t>Farbe des Tieres</t>
+  </si>
+  <si>
+    <t>Angebot</t>
+  </si>
+  <si>
+    <t>Rolle</t>
+  </si>
+  <si>
+    <t>Seitenzahl</t>
+  </si>
+  <si>
+    <t>Kurzer Name</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Zeitstempel</t>
+  </si>
+  <si>
+    <t>Gewicht</t>
+  </si>
+  <si>
+    <t>Wunderland Standort</t>
+  </si>
+  <si>
+    <t>Kastriert</t>
+  </si>
+  <si>
+    <t>Teil von</t>
+  </si>
+  <si>
+    <t>Link zu Alice Charakter</t>
+  </si>
+  <si>
+    <t>Link zum Tiercharakter</t>
+  </si>
+  <si>
+    <t>Link zum Tierfreund</t>
+  </si>
+  <si>
+    <t>Link zu Audio</t>
+  </si>
+  <si>
+    <t>Link zu Butler</t>
+  </si>
+  <si>
+    <t>Link zum Märchen</t>
+  </si>
+  <si>
+    <t>Link zum Bild</t>
+  </si>
+  <si>
+    <t>Link zum Standort</t>
+  </si>
+  <si>
+    <t>Link zum Video</t>
+  </si>
+  <si>
+    <t>Link zum Infoblatt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -720,17 +1054,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,21 +1280,21 @@
   <dimension ref="A1:Q942"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="12" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="1.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="1.83203125" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.1640625" customWidth="1"/>
     <col min="13" max="13" width="29.1640625" customWidth="1"/>
@@ -975,7 +1306,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1028,9 +1359,15 @@
       <c r="B2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -1038,10 +1375,10 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>82</v>
@@ -1056,8 +1393,17 @@
       <c r="B3" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
+        <v>181</v>
+      </c>
       <c r="L3" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>34</v>
@@ -1069,13 +1415,22 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="C4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" t="s">
+        <v>182</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>19</v>
@@ -1084,18 +1439,27 @@
         <v>20</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>17</v>
@@ -1107,17 +1471,26 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="C6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>184</v>
+      </c>
       <c r="L6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>82</v>
@@ -1125,12 +1498,21 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>126</v>
+      <c r="A7" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>185</v>
+      </c>
       <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1141,19 +1523,28 @@
         <v>20</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>186</v>
+      </c>
       <c r="L8" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>17</v>
@@ -1165,12 +1556,21 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>125</v>
+      <c r="A9" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>187</v>
+      </c>
       <c r="L9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1181,17 +1581,26 @@
         <v>20</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="C10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
       <c r="L10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1204,12 +1613,21 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="C11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" t="s">
+        <v>189</v>
+      </c>
       <c r="L11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1222,12 +1640,21 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" t="s">
+        <v>190</v>
+      </c>
       <c r="L12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1241,14 +1668,23 @@
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>191</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>19</v>
@@ -1257,17 +1693,26 @@
         <v>20</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
       <c r="L14" s="3" t="s">
         <v>16</v>
       </c>
@@ -1281,14 +1726,23 @@
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
       <c r="L15" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>17</v>
@@ -1296,16 +1750,25 @@
       <c r="N15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="P15" s="5"/>
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" t="s">
+        <v>192</v>
+      </c>
       <c r="L16" s="3" t="s">
         <v>30</v>
       </c>
@@ -1319,14 +1782,23 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" t="s">
+        <v>193</v>
+      </c>
       <c r="L17" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>19</v>
@@ -1335,18 +1807,27 @@
         <v>20</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" t="s">
+        <v>190</v>
+      </c>
       <c r="L18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1356,33 +1837,51 @@
       <c r="N18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="9"/>
+      <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="C19" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" t="s">
+        <v>194</v>
+      </c>
       <c r="L19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="C20" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" t="s">
+        <v>195</v>
+      </c>
       <c r="L20" s="3" t="s">
         <v>22</v>
       </c>
@@ -1396,12 +1895,21 @@
       <c r="Q20" s="3"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="C21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" t="s">
+        <v>196</v>
+      </c>
       <c r="L21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1414,12 +1922,21 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>123</v>
+      <c r="A22" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C22" t="s">
+        <v>232</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" t="s">
+        <v>197</v>
+      </c>
       <c r="L22" s="3" t="s">
         <v>16</v>
       </c>
@@ -1430,20 +1947,29 @@
         <v>20</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" t="s">
+        <v>198</v>
+      </c>
       <c r="L23" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>34</v>
@@ -1455,12 +1981,21 @@
       <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>124</v>
+      <c r="A24" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="C24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>199</v>
+      </c>
       <c r="L24" s="3" t="s">
         <v>16</v>
       </c>
@@ -1473,12 +2008,21 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>120</v>
+      <c r="A25" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="C25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
       <c r="L25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1489,18 +2033,27 @@
         <v>20</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="C26" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" t="s">
+        <v>200</v>
+      </c>
       <c r="L26" s="3" t="s">
         <v>16</v>
       </c>
@@ -1514,14 +2067,23 @@
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" t="s">
+        <v>201</v>
+      </c>
       <c r="L27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>25</v>
@@ -1533,14 +2095,23 @@
       <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="C28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" t="s">
+        <v>202</v>
+      </c>
       <c r="L28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>48</v>
@@ -1548,35 +2119,53 @@
       <c r="N28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P28" s="9"/>
+      <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="L29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N29" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="P29" s="3"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="C30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" t="s">
+        <v>203</v>
+      </c>
       <c r="L30" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>39</v>
@@ -1588,17 +2177,26 @@
       <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="C31" t="s">
+        <v>241</v>
+      </c>
+      <c r="D31" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" t="s">
+        <v>204</v>
+      </c>
       <c r="L31" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N31" s="3" t="s">
         <v>40</v>
@@ -1606,12 +2204,21 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="C32" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" t="s">
+        <v>205</v>
+      </c>
       <c r="L32" s="3" t="s">
         <v>41</v>
       </c>
@@ -1625,17 +2232,26 @@
       <c r="Q32" s="3"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="C33" t="s">
+        <v>243</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" t="s">
+        <v>206</v>
+      </c>
       <c r="L33" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>40</v>
@@ -1644,12 +2260,21 @@
       <c r="Q33" s="3"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="C34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" t="s">
+        <v>207</v>
+      </c>
       <c r="L34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1663,17 +2288,26 @@
       <c r="Q34" s="3"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="C35" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>208</v>
+      </c>
       <c r="L35" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N35" s="3" t="s">
         <v>40</v>
@@ -1681,11 +2315,20 @@
       <c r="P35" s="3"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" t="s">
+        <v>209</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>41</v>
@@ -1703,26 +2346,44 @@
       <c r="A37" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>109</v>
+      <c r="B37" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" t="s">
+        <v>210</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N37" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="C38" t="s">
+        <v>247</v>
+      </c>
+      <c r="D38" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" t="s">
+        <v>211</v>
+      </c>
       <c r="L38" s="3" t="s">
         <v>41</v>
       </c>
@@ -1736,17 +2397,26 @@
       <c r="Q38" s="3"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="C39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" t="s">
+        <v>212</v>
+      </c>
       <c r="L39" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N39" s="3" t="s">
         <v>40</v>
@@ -1754,11 +2424,20 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" t="s">
+        <v>213</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
update data model and add header
</commit_message>
<xml_diff>
--- a/data_model_files/daschland (daschland)/properties.xlsx
+++ b/data_model_files/daschland (daschland)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data_model_files/daschland (daschland)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data_model_files/daschland (daschland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEDF6DD-01F1-0947-8723-FE5630CB7CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B18812-187F-5144-A5C8-E9D4F3C2377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="500" windowWidth="59460" windowHeight="23880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,9 +629,6 @@
     <t>hasValue, schema:weight</t>
   </si>
   <si>
-    <t>hasValuem schema:location</t>
-  </si>
-  <si>
     <t>hasValue, schema:gender</t>
   </si>
   <si>
@@ -972,6 +969,9 @@
   </si>
   <si>
     <t>Link zum Infoblatt</t>
+  </si>
+  <si>
+    <t>hasValue, schema:location</t>
   </si>
 </sst>
 </file>
@@ -1279,9 +1279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q942"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1360,13 +1360,13 @@
         <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
@@ -1394,13 +1394,13 @@
         <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>132</v>
@@ -1421,13 +1421,13 @@
         <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>133</v>
@@ -1450,13 +1450,13 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>134</v>
@@ -1478,13 +1478,13 @@
         <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>16</v>
@@ -1508,10 +1508,10 @@
         <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>16</v>
@@ -1535,16 +1535,16 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>17</v>
@@ -1563,13 +1563,13 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>16</v>
@@ -1593,13 +1593,13 @@
         <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>16</v>
@@ -1620,13 +1620,13 @@
         <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>16</v>
@@ -1647,13 +1647,13 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>28</v>
@@ -1675,16 +1675,16 @@
         <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>19</v>
@@ -1742,7 +1742,7 @@
         <v>31</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>17</v>
@@ -1761,13 +1761,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>30</v>
@@ -1789,16 +1789,16 @@
         <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>19</v>
@@ -1823,10 +1823,10 @@
         <v>50</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>16</v>
@@ -1847,13 +1847,13 @@
         <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>16</v>
@@ -1874,13 +1874,13 @@
         <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>22</v>
@@ -1902,13 +1902,13 @@
         <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>16</v>
@@ -1929,13 +1929,13 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>16</v>
@@ -1960,16 +1960,16 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>34</v>
@@ -1988,13 +1988,13 @@
         <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>16</v>
@@ -2015,10 +2015,10 @@
         <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E25" t="s">
         <v>91</v>
@@ -2046,13 +2046,13 @@
         <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>16</v>
@@ -2074,13 +2074,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>135</v>
@@ -2102,16 +2102,16 @@
         <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E28" t="s">
-        <v>202</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>136</v>
+        <v>201</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>48</v>
@@ -2129,13 +2129,13 @@
         <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>16</v>
@@ -2156,16 +2156,16 @@
         <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>39</v>
@@ -2184,13 +2184,13 @@
         <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>41</v>
@@ -2211,13 +2211,13 @@
         <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>41</v>
@@ -2239,13 +2239,13 @@
         <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>41</v>
@@ -2267,13 +2267,13 @@
         <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>41</v>
@@ -2295,13 +2295,13 @@
         <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>41</v>
@@ -2322,13 +2322,13 @@
         <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>41</v>
@@ -2347,16 +2347,16 @@
         <v>108</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>41</v>
@@ -2376,13 +2376,13 @@
         <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>41</v>
@@ -2404,13 +2404,13 @@
         <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>41</v>
@@ -2431,13 +2431,13 @@
         <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>41</v>

</xml_diff>